<commit_message>
Edited english table by translating spanish portions
</commit_message>
<xml_diff>
--- a/Indicators/Indicators_Objectives.xlsx
+++ b/Indicators/Indicators_Objectives.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caio_Otto\Desktop\Bren School\TURFeffect\Docs\Indicators\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melai\Documents\GitHub\Docs\Indicators\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="19440" windowHeight="8010"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="19440" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Spanish" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="75">
   <si>
     <t xml:space="preserve">Objetivos </t>
   </si>
@@ -229,25 +229,28 @@
     <t>Recover species of economic interest</t>
   </si>
   <si>
-    <t>Conserve species under special protection regimen</t>
-  </si>
-  <si>
     <t>Improve fishery production in nearby waters</t>
   </si>
   <si>
     <t>Recover overexploited species</t>
   </si>
   <si>
-    <t>Contribute to maintain biological process (crianza, reclutamiento, crecimiento, reproducción, alimentación)</t>
-  </si>
-  <si>
     <t>Preserve biological diversity and the ecosystem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avoid overexploitation </t>
+  </si>
+  <si>
+    <t>Contribute to maintain biological process (reproduction, recruitment, growth, feeding)</t>
+  </si>
+  <si>
+    <t>Conserve species under a special protection regimen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -533,6 +536,63 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
@@ -548,71 +608,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -637,9 +640,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -677,7 +680,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -712,6 +715,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -747,9 +767,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -925,77 +962,77 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="63.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="63.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.81640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="63.42578125" style="1"/>
+    <col min="3" max="3" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="63.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+    <row r="1" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21" t="s">
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="22"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="41"/>
     </row>
-    <row r="3" spans="2:30" s="2" customFormat="1" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="37"/>
+    <row r="3" spans="2:30" s="2" customFormat="1" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="43"/>
       <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
@@ -1081,87 +1118,87 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="2:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B4" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="S4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="T4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="U4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="W4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="X4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD4" s="29" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD4" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="38" t="s">
+    <row r="5" spans="2:30" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="32" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="7"/>
@@ -1235,8 +1272,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="39" t="s">
+    <row r="6" spans="2:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="33" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="7"/>
@@ -1318,8 +1355,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="38" t="s">
+    <row r="7" spans="2:30" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="32" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7"/>
@@ -1403,8 +1440,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="39" t="s">
+    <row r="8" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B8" s="33" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="7"/>
@@ -1478,8 +1515,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:30" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="38" t="s">
+    <row r="9" spans="2:30" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B9" s="32" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -1555,84 +1592,84 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="41" t="s">
+    <row r="10" spans="2:30" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="S10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="T10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="U10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="V10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="W10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="X10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD10" s="36" t="s">
+      <c r="C10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="25"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="V10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="W10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="X10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD10" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
     </row>
   </sheetData>
@@ -1650,78 +1687,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AD11"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="63.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="63.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" style="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="19" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="3.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="16384" width="63.42578125" style="1"/>
+    <col min="3" max="3" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="19" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="30" width="6.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="16384" width="63.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="40" t="s">
+    <row r="1" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20" t="s">
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="21" t="s">
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
-      <c r="Y2" s="21"/>
-      <c r="Z2" s="21"/>
-      <c r="AA2" s="21"/>
-      <c r="AB2" s="21"/>
-      <c r="AC2" s="21"/>
-      <c r="AD2" s="22"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="40"/>
+      <c r="V2" s="40"/>
+      <c r="W2" s="40"/>
+      <c r="X2" s="40"/>
+      <c r="Y2" s="40"/>
+      <c r="Z2" s="40"/>
+      <c r="AA2" s="40"/>
+      <c r="AB2" s="40"/>
+      <c r="AC2" s="40"/>
+      <c r="AD2" s="41"/>
     </row>
-    <row r="3" spans="2:30" s="2" customFormat="1" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="42"/>
+    <row r="3" spans="2:30" s="2" customFormat="1" ht="96.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="44"/>
       <c r="C3" s="4" t="s">
         <v>41</v>
       </c>
@@ -1807,88 +1844,88 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B4" s="39" t="s">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="23"/>
-      <c r="G4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="24"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="O4" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="P4" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="R4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="S4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="T4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="U4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="V4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="W4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="X4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB4" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC4" s="27" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD4" s="29" t="s">
+      <c r="C4" s="19"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="18"/>
+      <c r="G4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="19"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="R4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="S4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="U4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="W4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="X4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD4" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="38" t="s">
-        <v>69</v>
+    <row r="5" spans="2:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="32" t="s">
+        <v>74</v>
       </c>
       <c r="C5" s="7"/>
       <c r="D5" s="11"/>
@@ -1961,9 +1998,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="43" t="s">
-        <v>70</v>
+    <row r="6" spans="2:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="11"/>
@@ -2044,9 +2081,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:30" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="38" t="s">
-        <v>4</v>
+    <row r="7" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B7" s="32" t="s">
+        <v>72</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="11"/>
@@ -2129,9 +2166,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B8" s="43" t="s">
-        <v>71</v>
+    <row r="8" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B8" s="35" t="s">
+        <v>70</v>
       </c>
       <c r="C8" s="7"/>
       <c r="D8" s="11"/>
@@ -2204,9 +2241,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:30" ht="60" x14ac:dyDescent="0.25">
-      <c r="B9" s="38" t="s">
-        <v>72</v>
+    <row r="9" spans="2:30" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>8</v>
@@ -2281,84 +2318,84 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:30" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="44" t="s">
-        <v>73</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" s="30"/>
-      <c r="H10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="J10" s="31" t="s">
-        <v>8</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="33"/>
-      <c r="N10" s="32"/>
-      <c r="O10" s="33"/>
-      <c r="P10" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="S10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="T10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="U10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="V10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="W10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="X10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB10" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC10" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD10" s="36" t="s">
+    <row r="10" spans="2:30" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="25"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="R10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="S10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="T10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="V10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="W10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="X10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD10" s="31" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split each indicator type into a separate table
because the table is too big to fit in the guidebook
</commit_message>
<xml_diff>
--- a/Indicators/Indicators_Objectives.xlsx
+++ b/Indicators/Indicators_Objectives.xlsx
@@ -9,18 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="19440" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="19440" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Spanish" sheetId="1" r:id="rId1"/>
     <sheet name="English" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="75">
   <si>
     <t xml:space="preserve">Objetivos </t>
   </si>
@@ -333,7 +335,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -479,11 +481,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
@@ -615,6 +648,75 @@
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1685,15 +1787,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:AD11"/>
+  <dimension ref="B1:AD41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33:P41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="63.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.453125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.7265625" style="1" bestFit="1" customWidth="1"/>
@@ -2398,14 +2500,1389 @@
     <row r="11" spans="2:30" x14ac:dyDescent="0.35">
       <c r="B11" s="3"/>
     </row>
+    <row r="12" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="13" spans="2:30" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="45"/>
+    </row>
+    <row r="14" spans="2:30" ht="88" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="44"/>
+      <c r="C14" s="46" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="I14" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" x14ac:dyDescent="0.35">
+      <c r="B15" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="50"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="19"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="51" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" ht="29" x14ac:dyDescent="0.35">
+      <c r="B16" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="52"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="11"/>
+      <c r="G16" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B17" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C17" s="52"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B18" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B19" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="52"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="11"/>
+      <c r="G19" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" s="52" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="K20" s="53"/>
+    </row>
+    <row r="21" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="54" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="25"/>
+      <c r="H21" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J21" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="55"/>
+    </row>
+    <row r="22" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="23" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="61"/>
+    </row>
+    <row r="24" spans="2:11" ht="187" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="44"/>
+      <c r="C24" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G24" s="59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B25" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B26" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="29" x14ac:dyDescent="0.35">
+      <c r="B27" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B28" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B29" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C29" s="64"/>
+      <c r="D29" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="8"/>
+      <c r="F29" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B30" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C30" s="64"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="8"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B31" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="66"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B33" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="40"/>
+      <c r="N33" s="40"/>
+      <c r="O33" s="40"/>
+      <c r="P33" s="41"/>
+    </row>
+    <row r="34" spans="2:16" ht="166" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B34" s="44"/>
+      <c r="C34" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K34" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M34" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O34" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="P34" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B35" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O35" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P35" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B36" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P36" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B37" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O37" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P37" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B38" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O38" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P38" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B39" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N39" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O39" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P39" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B40" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N40" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O40" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P40" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="K41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="N41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="O41" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="P41" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="10">
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="C33:P33"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:K2"/>
     <mergeCell ref="L2:P2"/>
     <mergeCell ref="Q2:AD2"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="C13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:G11"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="3.1796875" customWidth="1"/>
+    <col min="2" max="2" width="36.7265625" customWidth="1"/>
+    <col min="3" max="3" width="3.6328125" customWidth="1"/>
+    <col min="4" max="4" width="6.26953125" customWidth="1"/>
+    <col min="5" max="5" width="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="60" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="61"/>
+    </row>
+    <row r="4" spans="2:7" ht="82" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="44"/>
+      <c r="C4" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="58" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B6" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="B7" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="64"/>
+      <c r="D9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="49" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="64"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="67" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="37" customWidth="1"/>
+    <col min="3" max="3" width="3.54296875" customWidth="1"/>
+    <col min="4" max="4" width="5.81640625" customWidth="1"/>
+    <col min="5" max="5" width="8.54296875" customWidth="1"/>
+    <col min="6" max="6" width="3.36328125" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="5.6328125" customWidth="1"/>
+    <col min="10" max="10" width="3.36328125" customWidth="1"/>
+    <col min="11" max="11" width="5.81640625" customWidth="1"/>
+    <col min="14" max="14" width="3.08984375" customWidth="1"/>
+    <col min="15" max="15" width="5.7265625" customWidth="1"/>
+    <col min="16" max="16" width="5.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="40"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="41"/>
+    </row>
+    <row r="3" spans="2:16" ht="77" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="44"/>
+      <c r="C3" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="P3" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B4" s="33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="O4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B6" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O6" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P6" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B7" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O7" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P7" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="B8" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P8" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B9" s="32" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="O9" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="P9" s="17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="O10" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10" s="31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:P2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>